<commit_message>
chore(data): Update price, config and deal data
</commit_message>
<xml_diff>
--- a/prix_lego.xlsx
+++ b/prix_lego.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1178"/>
+  <dimension ref="A1:F1322"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -35111,6 +35111,4326 @@
         </is>
       </c>
     </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1179" t="n">
+        <v>45.97</v>
+      </c>
+      <c r="F1179" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123371</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1180" t="n">
+        <v>45.97</v>
+      </c>
+      <c r="F1180" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125909</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1181" t="n">
+        <v>45.97</v>
+      </c>
+      <c r="F1181" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122380</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1182" t="n">
+        <v>49.99</v>
+      </c>
+      <c r="F1182" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124002</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1183" t="n">
+        <v>49.99</v>
+      </c>
+      <c r="F1183" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123082</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1184" t="n">
+        <v>52.99</v>
+      </c>
+      <c r="F1184" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123408</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1185" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="F1185" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122283</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1186" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="F1186" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122875</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1187" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="F1187" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123673</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1188" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="F1188" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123548</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>10348</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>Bonsaï d’érable rouge du Japon</t>
+        </is>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1189" t="n">
+        <v>59.99</v>
+      </c>
+      <c r="F1189" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125478</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>10357</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>Shelby Cobra 427 SC</t>
+        </is>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1190" t="n">
+        <v>149.99</v>
+      </c>
+      <c r="F1190" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124280</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1191" t="n">
+        <v>149.97</v>
+      </c>
+      <c r="F1191" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124379</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1192" t="n">
+        <v>149.97</v>
+      </c>
+      <c r="F1192" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126832</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1193" t="n">
+        <v>149.97</v>
+      </c>
+      <c r="F1193" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125799</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1194" t="n">
+        <v>149.99</v>
+      </c>
+      <c r="F1194" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124202</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1195" t="n">
+        <v>166.04</v>
+      </c>
+      <c r="F1195" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125668</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1196" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1196" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/121684</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1197" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1197" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125984</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1198" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1198" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125690</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1199" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1199" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125657</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>72037</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>Mario Kart Mario et kart standard</t>
+        </is>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1200" t="n">
+        <v>185.49</v>
+      </c>
+      <c r="F1200" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125989</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1201" t="n">
+        <v>75.20999999999999</v>
+      </c>
+      <c r="F1201" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/83067</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1202" t="n">
+        <v>75.20999999999999</v>
+      </c>
+      <c r="F1202" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/84303</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1203" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1203" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/91282</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1204" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1204" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/83015</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1205" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1205" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/90181</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1206" t="n">
+        <v>90.98999999999999</v>
+      </c>
+      <c r="F1206" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/84555</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1207" t="n">
+        <v>93.26000000000001</v>
+      </c>
+      <c r="F1207" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/83457</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1208" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1208" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/83008</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1209" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1209" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/83502</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1210" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1210" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1210" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/95703</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>10298</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>Vespa 125</t>
+        </is>
+      </c>
+      <c r="D1211" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1211" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1211" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124612</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1212" t="n">
+        <v>339.99</v>
+      </c>
+      <c r="F1212" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114139</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1213" t="n">
+        <v>339.99</v>
+      </c>
+      <c r="F1213" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114156</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1214" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1214" t="n">
+        <v>339.99</v>
+      </c>
+      <c r="F1214" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112815</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1215" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1215" t="n">
+        <v>349.99</v>
+      </c>
+      <c r="F1215" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114104</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1216" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1216" t="n">
+        <v>360.99</v>
+      </c>
+      <c r="F1216" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113684</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1217" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1217" t="n">
+        <v>399</v>
+      </c>
+      <c r="F1217" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125143</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1218" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1218" t="n">
+        <v>399.99</v>
+      </c>
+      <c r="F1218" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/115791</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1219" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1219" t="n">
+        <v>418.99</v>
+      </c>
+      <c r="F1219" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114146</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1220" t="n">
+        <v>449.99</v>
+      </c>
+      <c r="F1220" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112662</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1221" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1221" t="n">
+        <v>449.99</v>
+      </c>
+      <c r="F1221" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114159</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>42172</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>McLaren P1</t>
+        </is>
+      </c>
+      <c r="D1222" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1222" t="n">
+        <v>449.99</v>
+      </c>
+      <c r="F1222" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/114136</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1223" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1223" t="n">
+        <v>109.99</v>
+      </c>
+      <c r="F1223" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127215</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1224" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1224" t="n">
+        <v>109.99</v>
+      </c>
+      <c r="F1224" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127410</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1225" t="n">
+        <v>128.99</v>
+      </c>
+      <c r="F1225" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127269</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1226" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1226" t="n">
+        <v>129.99</v>
+      </c>
+      <c r="F1226" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123975</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1227" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1227" t="n">
+        <v>129.99</v>
+      </c>
+      <c r="F1227" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127339</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1228" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1228" t="n">
+        <v>129.99</v>
+      </c>
+      <c r="F1228" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127293</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>75639</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>Le bateau pirate Vogue Merry</t>
+        </is>
+      </c>
+      <c r="D1229" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1229" t="n">
+        <v>129.99</v>
+      </c>
+      <c r="F1229" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127222</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>10375</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>Dragons Krokmou</t>
+        </is>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1230" t="n">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="F1230" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123824</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>10375</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>Dragons Krokmou</t>
+        </is>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1231" t="n">
+        <v>95.98999999999999</v>
+      </c>
+      <c r="F1231" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127216</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>10289</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>Oiseau de paradis</t>
+        </is>
+      </c>
+      <c r="D1232" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1232" t="n">
+        <v>283</v>
+      </c>
+      <c r="F1232" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/76315</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>10289</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>Oiseau de paradis</t>
+        </is>
+      </c>
+      <c r="D1233" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1233" t="n">
+        <v>299.99</v>
+      </c>
+      <c r="F1233" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/79992</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>10372</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>Hibiscus</t>
+        </is>
+      </c>
+      <c r="D1234" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1234" t="n">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="F1234" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125696</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>10372</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>Hibiscus</t>
+        </is>
+      </c>
+      <c r="D1235" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1235" t="n">
+        <v>69.98999999999999</v>
+      </c>
+      <c r="F1235" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126852</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>10372</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>Hibiscus</t>
+        </is>
+      </c>
+      <c r="D1236" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1236" t="n">
+        <v>95.98999999999999</v>
+      </c>
+      <c r="F1236" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/127075</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1237" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1237" t="n">
+        <v>79.98999999999999</v>
+      </c>
+      <c r="F1237" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100568</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1238" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1238" t="n">
+        <v>90.34999999999999</v>
+      </c>
+      <c r="F1238" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/98393</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1239" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1239" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1239" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/98666</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1240" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1240" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/101441</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1241" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1241" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1241" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112532</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1242" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1242" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100356</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1243" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1243" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124770</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1244" t="n">
+        <v>102.99</v>
+      </c>
+      <c r="F1244" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100058</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1245" t="n">
+        <v>108.99</v>
+      </c>
+      <c r="F1245" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100101</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1246" t="n">
+        <v>19.52</v>
+      </c>
+      <c r="F1246" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113311</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1247" t="n">
+        <v>19.52</v>
+      </c>
+      <c r="F1247" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112455</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1248" t="n">
+        <v>19.52</v>
+      </c>
+      <c r="F1248" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112557</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1249" t="n">
+        <v>24.99</v>
+      </c>
+      <c r="F1249" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112445</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1250" t="n">
+        <v>25.99</v>
+      </c>
+      <c r="F1250" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112272</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1251" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1251" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/112442</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1252" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1252" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113695</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1253" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1253" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113352</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1254" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1254" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113938</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1255" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1255" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/113919</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>10368</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>Le chrysanthème</t>
+        </is>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1256" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F1256" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125125</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1257" t="n">
+        <v>47.39</v>
+      </c>
+      <c r="F1257" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123376</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1258" t="n">
+        <v>47.39</v>
+      </c>
+      <c r="F1258" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125854</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1259" t="n">
+        <v>47.39</v>
+      </c>
+      <c r="F1259" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122740</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1260" t="n">
+        <v>56.99</v>
+      </c>
+      <c r="F1260" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1261" t="n">
+        <v>57.99</v>
+      </c>
+      <c r="F1261" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123103</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1262" t="n">
+        <v>58.99</v>
+      </c>
+      <c r="F1262" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124287</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1263" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1263" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122404</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1264" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1264" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122851</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1265" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1265" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123677</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1266" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1266" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123540</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>43257</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>Angel</t>
+        </is>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1267" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1267" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125521</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1268" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1268" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126930</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1269" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1269" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126389</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1270" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1270" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126127</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1271" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1271" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125648</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1272" t="n">
+        <v>169.99</v>
+      </c>
+      <c r="F1272" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125809</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1273" t="n">
+        <v>188.99</v>
+      </c>
+      <c r="F1273" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126375</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1274" t="n">
+        <v>191.39</v>
+      </c>
+      <c r="F1274" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126547</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1275" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="F1275" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125769</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1276" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="F1276" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126572</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>75417</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>Le marcheur AT-ST™</t>
+        </is>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1277" t="n">
+        <v>199.99</v>
+      </c>
+      <c r="F1277" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126457</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1278" t="n">
+        <v>94.89</v>
+      </c>
+      <c r="F1278" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123460</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1279" t="n">
+        <v>94.89</v>
+      </c>
+      <c r="F1279" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125853</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1280" t="n">
+        <v>94.89</v>
+      </c>
+      <c r="F1280" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123638</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1281" t="n">
+        <v>94.98999999999999</v>
+      </c>
+      <c r="F1281" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1282" t="n">
+        <v>113.49</v>
+      </c>
+      <c r="F1282" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124309</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1283" t="n">
+        <v>114.99</v>
+      </c>
+      <c r="F1283" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123116</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1284" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F1284" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122538</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1285" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F1285" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122893</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1286" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F1286" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123695</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1287" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F1287" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/123544</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>43267</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>Le château des princesses et les animaux royaux</t>
+        </is>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1288" t="n">
+        <v>119.99</v>
+      </c>
+      <c r="F1288" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125520</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1289" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1289" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126354</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1290" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1290" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125735</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1291" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1291" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126781</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1292" t="n">
+        <v>64.98999999999999</v>
+      </c>
+      <c r="F1292" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126681</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1293" t="n">
+        <v>74.98999999999999</v>
+      </c>
+      <c r="F1293" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126940</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1294" t="n">
+        <v>80.98999999999999</v>
+      </c>
+      <c r="F1294" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126029</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1295" t="n">
+        <v>89.73999999999999</v>
+      </c>
+      <c r="F1295" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126542</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1296" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1296" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122476</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1297" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1297" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126592</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1298" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1298" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/126466</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>31167</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>Le manoir hanté</t>
+        </is>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1299" t="n">
+        <v>89.98999999999999</v>
+      </c>
+      <c r="F1299" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125581</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1300" t="n">
+        <v>69.90000000000001</v>
+      </c>
+      <c r="F1300" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100547</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1301" t="n">
+        <v>72.17</v>
+      </c>
+      <c r="F1301" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100108</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1302" t="n">
+        <v>72.17</v>
+      </c>
+      <c r="F1302" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100049</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1303" t="n">
+        <v>72.17</v>
+      </c>
+      <c r="F1303" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100169</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1304" t="n">
+        <v>76.98999999999999</v>
+      </c>
+      <c r="F1304" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/104138</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1305" t="n">
+        <v>80.98999999999999</v>
+      </c>
+      <c r="F1305" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100364</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1306" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1306" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/97159</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1307" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1307" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/100066</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1308" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1308" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/102495</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1309" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1309" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/110235</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>60367</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>L’avion de ligne</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1310" t="n">
+        <v>99.98999999999999</v>
+      </c>
+      <c r="F1310" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/124771</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>Cdiscount</t>
+        </is>
+      </c>
+      <c r="E1311" t="n">
+        <v>17.99</v>
+      </c>
+      <c r="F1311" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/120632</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1312" t="inlineStr">
+        <is>
+          <t>Leclerc</t>
+        </is>
+      </c>
+      <c r="E1312" t="n">
+        <v>17.99</v>
+      </c>
+      <c r="F1312" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/120893</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1313" t="inlineStr">
+        <is>
+          <t>Amazon</t>
+        </is>
+      </c>
+      <c r="E1313" t="n">
+        <v>17.99</v>
+      </c>
+      <c r="F1313" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/116193</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1314" t="inlineStr">
+        <is>
+          <t>KidInn</t>
+        </is>
+      </c>
+      <c r="E1314" t="n">
+        <v>22.99</v>
+      </c>
+      <c r="F1314" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/121272</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1315" t="inlineStr">
+        <is>
+          <t>Fnac</t>
+        </is>
+      </c>
+      <c r="E1315" t="n">
+        <v>22.99</v>
+      </c>
+      <c r="F1315" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/120116</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1316" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1316" t="n">
+        <v>22.99</v>
+      </c>
+      <c r="F1316" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/120774</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1317" t="inlineStr">
+        <is>
+          <t>Carrefour</t>
+        </is>
+      </c>
+      <c r="E1317" t="n">
+        <v>24.99</v>
+      </c>
+      <c r="F1317" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/121197</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1318" t="inlineStr">
+        <is>
+          <t>Lego</t>
+        </is>
+      </c>
+      <c r="E1318" t="n">
+        <v>26.99</v>
+      </c>
+      <c r="F1318" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/116211</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1319" t="inlineStr">
+        <is>
+          <t>La Grande Récré</t>
+        </is>
+      </c>
+      <c r="E1319" t="n">
+        <v>26.99</v>
+      </c>
+      <c r="F1319" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/122187</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1320" t="inlineStr">
+        <is>
+          <t>JouéClub</t>
+        </is>
+      </c>
+      <c r="E1320" t="n">
+        <v>26.99</v>
+      </c>
+      <c r="F1320" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/121408</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:05</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>77243</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>Voiture F1® Oracle Red Bull Racing RB20</t>
+        </is>
+      </c>
+      <c r="D1321" t="inlineStr">
+        <is>
+          <t>Ltoys</t>
+        </is>
+      </c>
+      <c r="E1321" t="n">
+        <v>26.99</v>
+      </c>
+      <c r="F1321" t="inlineStr">
+        <is>
+          <t>https://www.avenuedelabrique.com/go/px/125226</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>2025-09-19 08:42:14</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>43230</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>La caméra Hommage à Walt Disney</t>
+        </is>
+      </c>
+      <c r="D1322" t="inlineStr">
+        <is>
+          <t>Auchan</t>
+        </is>
+      </c>
+      <c r="E1322" t="n">
+        <v>114.61</v>
+      </c>
+      <c r="F1322" t="inlineStr">
+        <is>
+          <t>https://www.auchan.fr/lego-lego-disney-43230-la-camera-hommage-a-walt-disney-maquette-pour-adultes-avec-mickey-et-minnie-mouse/pr-C1718290</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>